<commit_message>
finish 2kr and added first experiment (easy game mode)
-finished 2kr anaylisis (also excel charts)
-added firs experiment on easy game mode configuration (also excel chart)
</commit_message>
<xml_diff>
--- a/Analysis/2kr_analysis/boss_arrival_time_20-25/waiting_time/easy_game_mode/2kr_easy_game_mode_LOG_minon_waiting_time.xlsx
+++ b/Analysis/2kr_analysis/boss_arrival_time_20-25/waiting_time/easy_game_mode/2kr_easy_game_mode_LOG_minon_waiting_time.xlsx
@@ -851,1223 +851,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Constant std Test (Homoskedasticity)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$X$69:$X$228</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>0.396277625791835</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.401942646826349</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.851516139160089</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.901583355088922</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.279535389260841</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.280723692983158</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.614686050957381</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.655208713579925</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.82486193008782</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.830023541384187</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.23415850475039</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.27835329639343</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.777795071874892</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.77888835986378</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.03234383966493</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.05360829117849</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.199562696538351</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.204515310293449</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.677257959841565</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.723804786921791</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.118050027447239</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.119990257345878</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.530273048734031</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.573974361381267</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.57791824232486</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.579178022169106</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.989140560096299</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.02804138982678</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.573658301476543</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.574587223822159</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.866269499777462</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.897544824785731</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.396277625791835</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.401942646826349</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.851516139160089</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.901583355088922</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.279535389260841</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.280723692983158</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.614686050957381</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.655208713579925</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.82486193008782</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.830023541384187</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.23415850475039</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.27835329639343</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.777795071874892</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.77888835986378</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.03234383966493</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.05360829117849</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.199562696538351</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.204515310293449</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.677257959841565</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.723804786921791</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.118050027447239</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.119990257345878</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.530273048734031</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.573974361381267</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.57791824232486</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.579178022169106</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.989140560096299</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.02804138982678</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.573658301476543</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.574587223822159</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.866269499777462</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.897544824785731</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.396277625791835</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.401942646826349</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.851516139160089</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.901583355088922</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.279535389260841</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.280723692983158</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.614686050957381</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.655208713579925</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.82486193008782</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.830023541384187</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1.23415850475039</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.27835329639343</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.777795071874892</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.77888835986378</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1.03234383966493</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1.05360829117849</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.199562696538351</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.204515310293449</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.677257959841565</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.723804786921791</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.118050027447239</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.119990257345878</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.530273048734031</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.573974361381267</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.57791824232486</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.579178022169106</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.989140560096299</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.02804138982678</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.573658301476543</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.574587223822159</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.866269499777462</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.897544824785731</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.396277625791835</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.401942646826349</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.851516139160089</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.901583355088922</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.279535389260841</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.280723692983158</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.614686050957381</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.655208713579925</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.82486193008782</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.830023541384187</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>1.23415850475039</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>1.27835329639343</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.777795071874892</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.77888835986378</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>1.03234383966493</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>1.05360829117849</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.199562696538351</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.204515310293449</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.677257959841565</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.723804786921791</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.118050027447239</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.119990257345878</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.530273048734031</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.573974361381267</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.57791824232486</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.579178022169106</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.989140560096299</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>1.02804138982678</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.573658301476543</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.574587223822159</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.866269499777462</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.897544824785731</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.396277625791835</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0.401942646826349</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.851516139160089</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.901583355088922</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.279535389260841</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.280723692983158</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.614686050957381</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.655208713579925</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.82486193008782</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0.830023541384187</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1.23415850475039</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1.27835329639343</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.777795071874892</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.77888835986378</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1.03234383966493</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1.05360829117849</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.199562696538351</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.204515310293449</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.677257959841565</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.723804786921791</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.118050027447239</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.119990257345878</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.530273048734031</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.573974361381267</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.57791824232486</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.579178022169106</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.989140560096299</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>1.02804138982678</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.573658301476543</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.574587223822159</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.866269499777462</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>0.897544824785731</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Y$69:$Y$228</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>-0.150822616468583</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.153047423156565</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.0809390863684936</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.062255182452982</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.218378608438155</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.218050693998993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.215128937360357</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.17649084184331</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0323898566521446</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0366339945082412</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.02386669840997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.013675295862364</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.00798714729062722</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.00616286719937709</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.0522676532428938</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.0669135509059663</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-0.150016234772541</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.143526278085725</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.145240994062557</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-0.129636129088887</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-0.0897935869106779</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-0.0868545753092957</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-0.040763415292568</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-0.0333681975407843</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-0.163486394171899</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-0.164438323845615</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-0.127809500130351</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-0.12630687589204</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.028536858207362</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0304428464866774</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.100758771914736</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.106736729097717</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-0.144160866162028</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-0.130362444338598</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-0.024163111928402</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-0.00513106022558174</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-0.0816560237918759</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-0.0821910887574716</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-0.0706848931488163</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-0.0789200195640846</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>-0.188418600152064</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-0.180080358209321</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>-0.0715978576205909</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>-0.0475485325472442</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>-0.176472926039718</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-0.175859517654045</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-0.21262204940114</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-0.196084262247247</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-0.068091100796491</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-0.0701473589883733</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-0.00406015118256575</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-0.0120790868386983</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-0.0626097807928791</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-0.0614145500874529</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0520815935534834</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0388942860242452</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-0.0795483186597875</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-0.0792273399730099</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-0.116403303592726</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>-0.127248224834585</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-0.1605947529967</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>-0.158757505546412</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-0.0201069150739729</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>-0.0054082305704074</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.297491276750703</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.294025705452781</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.27394443322692</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.273998029591605</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.162426261453623</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.162980889708677</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.227240031741232</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.21104769601089</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.223890418537456</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.220256592117814</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.283416961084561</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.286398203086507</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0592053449491696</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.058290579749616</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.182634819477501</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.202671903847641</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.250141196742507</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.24831059305547</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.202084299751765</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.204339562202433</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.155582916919259</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.154468216181384</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.117737794228471</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.106022826927315</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.245728857358013</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.24590616431719</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.271958334074008</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.278734022013409</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.206168343998787</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.203642952483514</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0821749530237036</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0890640143790033</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0360734348809227</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0315464834183665</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>-0.0705979927677095</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-0.0979018249719902</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.137437157099877</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.13796518880227</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0598115034106897</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0437144351924679</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.00593087559731542</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.000857979286032151</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>-0.137557991186623</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>-0.163276778540513</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0659232999940669</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0649149386175891</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>-0.0327126573500175</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>-0.0431550721967098</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0673563283911476</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0686012908243868</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.00344219253737221</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>-0.00711695209031293</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.107087466865034</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.106008155194739</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-0.0285819797040212</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>-0.0367944082726995</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.120296192755294</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.119913806857598</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0723873539156651</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0600541592985364</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.087297665142666</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0870087432739516</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>-0.0148559370781942</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>-0.0219033982005568</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>-0.0385812290010155</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>-0.0421623213759837</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>-0.0982442421623159</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>-0.108709961941051</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.000171213676530502</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>-0.000704295754482109</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>-0.00123770464274786</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.000648730204036552</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>-0.0737925506348515</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>-0.0776682077027668</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-0.0503944138673764</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>-0.0618975961363846</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.0593314283871084</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.058816866486217</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.114967540516551</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.103480981502283</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>-0.0993901895646229</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>-0.103238246805759</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>-0.0562253470440137</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>-0.0555073941845347</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>-0.110267016080736</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>-0.112207245979375</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>-0.100473992785366</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>-0.0747545071380762</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>-0.12299033728162</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>-0.122154307356164</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>-0.100132884266595</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>-0.0852330805853205</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>-0.161408114352115</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>-0.162337036697731</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>-0.147970872786273</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-0.168489114705756</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="43081486"/>
-        <c:axId val="30033757"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="43081486"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Predicted Response</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="30033757"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="30033757"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Residuals</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="43081486"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2157,8 +941,8 @@
             <c:trendlineType val="linear"/>
             <c:forward val="0"/>
             <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3140,11 +1924,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44614701"/>
-        <c:axId val="97636552"/>
+        <c:axId val="8916218"/>
+        <c:axId val="2787431"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44614701"/>
+        <c:axId val="8916218"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3200,12 +1984,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97636552"/>
+        <c:crossAx val="2787431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97636552"/>
+        <c:axId val="2787431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3270,8 +2054,1224 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44614701"/>
+        <c:crossAx val="8916218"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Constant std Test (Homoskedasticity)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$69:$X$228</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>0.396277625791835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.401942646826349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.851516139160089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.901583355088922</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.279535389260841</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.280723692983158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.614686050957381</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.655208713579925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82486193008782</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.830023541384187</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.23415850475039</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.27835329639343</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.777795071874892</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.77888835986378</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.03234383966493</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.05360829117849</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.199562696538351</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.204515310293449</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.677257959841565</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.723804786921791</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.118050027447239</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.119990257345878</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.530273048734031</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.573974361381267</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.57791824232486</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.579178022169106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.989140560096299</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.02804138982678</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.573658301476543</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.574587223822159</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.866269499777462</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.897544824785731</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.396277625791835</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.401942646826349</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.851516139160089</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.901583355088922</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.279535389260841</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.280723692983158</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.614686050957381</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.655208713579925</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.82486193008782</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.830023541384187</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.23415850475039</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.27835329639343</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.777795071874892</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.77888835986378</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.03234383966493</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.05360829117849</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.199562696538351</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.204515310293449</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.677257959841565</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.723804786921791</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.118050027447239</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.119990257345878</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.530273048734031</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.573974361381267</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.57791824232486</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.579178022169106</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.989140560096299</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.02804138982678</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.573658301476543</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.574587223822159</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.866269499777462</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.897544824785731</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.396277625791835</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.401942646826349</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.851516139160089</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.901583355088922</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.279535389260841</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.280723692983158</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.614686050957381</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.655208713579925</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.82486193008782</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.830023541384187</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.23415850475039</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.27835329639343</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.777795071874892</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77888835986378</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.03234383966493</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.05360829117849</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.199562696538351</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.204515310293449</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.677257959841565</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.723804786921791</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.118050027447239</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.119990257345878</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.530273048734031</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.573974361381267</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.57791824232486</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.579178022169106</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.989140560096299</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.02804138982678</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.573658301476543</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.574587223822159</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.866269499777462</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.897544824785731</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.396277625791835</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.401942646826349</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.851516139160089</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.901583355088922</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.279535389260841</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.280723692983158</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.614686050957381</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.655208713579925</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.82486193008782</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.830023541384187</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.23415850475039</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.27835329639343</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.777795071874892</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.77888835986378</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.03234383966493</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.05360829117849</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.199562696538351</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.204515310293449</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.677257959841565</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.723804786921791</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.118050027447239</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.119990257345878</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.530273048734031</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.573974361381267</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.57791824232486</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.579178022169106</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.989140560096299</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.02804138982678</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.573658301476543</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.574587223822159</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.866269499777462</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.897544824785731</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.396277625791835</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.401942646826349</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.851516139160089</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.901583355088922</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.279535389260841</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.280723692983158</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.614686050957381</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.655208713579925</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.82486193008782</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.830023541384187</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1.23415850475039</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.27835329639343</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.777795071874892</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.77888835986378</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.03234383966493</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.05360829117849</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.199562696538351</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.204515310293449</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.677257959841565</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.723804786921791</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.118050027447239</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.119990257345878</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.530273048734031</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.573974361381267</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.57791824232486</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.579178022169106</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.989140560096299</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1.02804138982678</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.573658301476543</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.574587223822159</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.866269499777462</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.897544824785731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$69:$Y$228</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>-0.150822616468583</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.153047423156565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.0809390863684936</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.062255182452982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.218378608438155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.218050693998993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.215128937360357</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.17649084184331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0323898566521446</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0366339945082412</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.02386669840997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.013675295862364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.00798714729062722</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.00616286719937709</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.0522676532428938</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.0669135509059663</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.150016234772541</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.143526278085725</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.145240994062557</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.129636129088887</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.0897935869106779</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.0868545753092957</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.040763415292568</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.0333681975407843</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.163486394171899</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.164438323845615</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.127809500130351</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.12630687589204</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.028536858207362</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.0304428464866774</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.100758771914736</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.106736729097717</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.144160866162028</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.130362444338598</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.024163111928402</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.00513106022558174</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.0816560237918759</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.0821910887574716</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.0706848931488163</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.0789200195640846</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.188418600152064</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.180080358209321</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.0715978576205909</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.0475485325472442</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.176472926039718</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.175859517654045</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.21262204940114</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.196084262247247</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.068091100796491</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.0701473589883733</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.00406015118256575</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-0.0120790868386983</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-0.0626097807928791</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.0614145500874529</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.0520815935534834</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.0388942860242452</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.0795483186597875</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.0792273399730099</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.116403303592726</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.127248224834585</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.1605947529967</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.158757505546412</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-0.0201069150739729</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-0.0054082305704074</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.297491276750703</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.294025705452781</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.27394443322692</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.273998029591605</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.162426261453623</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.162980889708677</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.227240031741232</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.21104769601089</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.223890418537456</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.220256592117814</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.283416961084561</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.286398203086507</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.0592053449491696</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.058290579749616</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.182634819477501</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.202671903847641</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.250141196742507</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.24831059305547</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.202084299751765</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.204339562202433</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.155582916919259</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.154468216181384</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.117737794228471</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.106022826927315</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.245728857358013</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.24590616431719</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.271958334074008</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.278734022013409</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.206168343998787</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.203642952483514</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.0821749530237036</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.0890640143790033</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.0360734348809227</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.0315464834183665</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.0705979927677095</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.0979018249719902</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.137437157099877</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.13796518880227</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.0598115034106897</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.0437144351924679</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.00593087559731542</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.000857979286032151</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-0.137557991186623</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-0.163276778540513</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.0659232999940669</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.0649149386175891</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-0.0327126573500175</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-0.0431550721967098</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.0673563283911476</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.0686012908243868</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.00344219253737221</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-0.00711695209031293</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.107087466865034</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.106008155194739</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-0.0285819797040212</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-0.0367944082726995</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.120296192755294</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.119913806857598</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.0723873539156651</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.0600541592985364</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.087297665142666</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.0870087432739516</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>-0.0148559370781942</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>-0.0219033982005568</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-0.0385812290010155</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-0.0421623213759837</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-0.0982442421623159</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-0.108709961941051</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.000171213676530502</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-0.000704295754482109</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-0.00123770464274786</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.000648730204036552</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-0.0737925506348515</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-0.0776682077027668</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-0.0503944138673764</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-0.0618975961363846</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.0593314283871084</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.058816866486217</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.114967540516551</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.103480981502283</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>-0.0993901895646229</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-0.103238246805759</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-0.0562253470440137</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>-0.0555073941845347</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>-0.110267016080736</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>-0.112207245979375</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-0.100473992785366</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-0.0747545071380762</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-0.12299033728162</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-0.122154307356164</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-0.100132884266595</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-0.0852330805853205</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-0.161408114352115</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-0.162337036697731</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-0.147970872786273</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-0.168489114705756</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="81146280"/>
+        <c:axId val="73236806"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81146280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Predicted Response</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73236806"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73236806"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81146280"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3308,9 +3308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
+      <xdr:colOff>150480</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3318,8 +3318,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9772560" y="11727720"/>
-        <a:ext cx="7655040" cy="4548240"/>
+        <a:off x="9774000" y="11727720"/>
+        <a:ext cx="7667280" cy="4547880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3338,9 +3338,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>172800</xdr:colOff>
+      <xdr:colOff>172440</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3348,8 +3348,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26703000" y="11629800"/>
-        <a:ext cx="7073280" cy="4131720"/>
+        <a:off x="26728560" y="11629800"/>
+        <a:ext cx="7084080" cy="4131360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3369,11 +3369,11 @@
   </sheetPr>
   <dimension ref="A1:BP229"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U71" activeCellId="0" sqref="U71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H70" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S77" activeCellId="0" sqref="S77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>

</xml_diff>